<commit_message>
Atualização do arquivo de docs PGTWEB
</commit_message>
<xml_diff>
--- a/02_contPGT.xlsx
+++ b/02_contPGT.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G212"/>
+  <dimension ref="A1:G215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -704,7 +704,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Análise para regularização</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -724,7 +724,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>7A7091058DBBDBDBFFEC38A46A34A73F</t>
+          <t>A302966FBEB8741A989E30E3C1DB84A1</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -741,7 +741,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Solicitação de documentação complementar</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -761,10 +761,14 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>7DE34ABB18DFC4184EA4ECFE7822F34E</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
+          <t>7A7091058DBBDBDBFFEC38A46A34A73F</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Regularização</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr">
         <is>
           <t>Não</t>
@@ -774,7 +778,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Solicitação de documentação complementar</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -789,19 +793,15 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Andiara</t>
+          <t>Adrian</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1E28611DB40D7BCF9AF123CC4CC60BFE</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Regularização</t>
-        </is>
-      </c>
+          <t>7DE34ABB18DFC4184EA4ECFE7822F34E</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
           <t>Não</t>
@@ -811,7 +811,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Solicitação de documentação complementar</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -831,10 +831,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>069ACF289074156352A4781DFCD0D264</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
+          <t>1E28611DB40D7BCF9AF123CC4CC60BFE</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Regularização</t>
+        </is>
+      </c>
       <c r="G12" t="inlineStr">
         <is>
           <t>Não</t>
@@ -844,7 +848,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Solicitação de documentação complementar</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -859,19 +863,15 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Claudineia</t>
+          <t>Andiara</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>58258FAC18CC8DE705C5107FC0A0B759</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Regularização</t>
-        </is>
-      </c>
+          <t>069ACF289074156352A4781DFCD0D264</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
           <t>Não</t>
@@ -881,7 +881,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Solicitação de documentação complementar</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -901,10 +901,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>AF93B4687B22186B9F40FA9CAF59355D</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr"/>
+          <t>58258FAC18CC8DE705C5107FC0A0B759</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Regularização</t>
+        </is>
+      </c>
       <c r="G14" t="inlineStr">
         <is>
           <t>Não</t>
@@ -914,7 +918,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Análise para regularização</t>
+          <t>Solicitação de documentação complementar</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -929,19 +933,15 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Cristiane</t>
+          <t>Claudineia</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>180B234A9A4D11A43083BF6E6BFF3617</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Regularização</t>
-        </is>
-      </c>
+          <t>AF93B4687B22186B9F40FA9CAF59355D</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
           <t>Não</t>
@@ -951,7 +951,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Análise para regularização</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -971,7 +971,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>5AB0DA0076CB4A7BC654C14601170805</t>
+          <t>180B234A9A4D11A43083BF6E6BFF3617</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -988,7 +988,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização (2º Relatório)</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1008,7 +1008,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>B44DAF5094FF26D7D29600F23051E9C7</t>
+          <t>5AB0DA0076CB4A7BC654C14601170805</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1018,14 +1018,14 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Solicitação de documentação complementar</t>
+          <t>Relatório de conformidades para regularização (2º Relatório)</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1045,20 +1045,24 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0B020F956312AEDBA007ECBA724ED40B</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr"/>
+          <t>B44DAF5094FF26D7D29600F23051E9C7</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Regularização</t>
+        </is>
+      </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Solicitação de documentação complementar</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1073,19 +1077,15 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Debora</t>
+          <t>Cristiane</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>874465517EEF60A1E4B3C3E4DBF99215</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Regularização</t>
-        </is>
-      </c>
+          <t>0B020F956312AEDBA007ECBA724ED40B</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
           <t>Não</t>
@@ -1095,7 +1095,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Solicitação de documentação complementar</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1115,10 +1115,14 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>25B5DA7A79DCC134ADF32C921CBAB522</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr"/>
+          <t>874465517EEF60A1E4B3C3E4DBF99215</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Regularização</t>
+        </is>
+      </c>
       <c r="G20" t="inlineStr">
         <is>
           <t>Não</t>
@@ -1128,7 +1132,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Análise para regularização</t>
+          <t>Solicitação de documentação complementar</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1143,19 +1147,15 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Gabriel</t>
+          <t>Debora</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>962E98FB0F61D261DB0D48C557F70ED2</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Regularização</t>
-        </is>
-      </c>
+          <t>25B5DA7A79DCC134ADF32C921CBAB522</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
           <t>Não</t>
@@ -1165,7 +1165,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Análise para regularização</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1185,7 +1185,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>9D159FDA14EB647768A2EF8FCA866AF5</t>
+          <t>962E98FB0F61D261DB0D48C557F70ED2</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1202,7 +1202,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização (2º Relatório)</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1222,7 +1222,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>42A275CFB3A429A9CA6E7AB9FB7521B6</t>
+          <t>9D159FDA14EB647768A2EF8FCA866AF5</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1232,14 +1232,14 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Solicitação de documentação complementar</t>
+          <t>Relatório de conformidades para regularização (2º Relatório)</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1259,20 +1259,24 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>912B181376702376839E92A34234AB6F</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr"/>
+          <t>42A275CFB3A429A9CA6E7AB9FB7521B6</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Regularização</t>
+        </is>
+      </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Solicitação de documentação complementar</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1287,19 +1291,15 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Juliana</t>
+          <t>Gabriel</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>916E2681C0054750A9E687574A0B6489</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Regularização</t>
-        </is>
-      </c>
+          <t>912B181376702376839E92A34234AB6F</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
           <t>Não</t>
@@ -1309,7 +1309,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Solicitação de documentação complementar</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1329,10 +1329,14 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>F17621921D038A38C3EB0D53E3733F98</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr"/>
+          <t>916E2681C0054750A9E687574A0B6489</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Regularização</t>
+        </is>
+      </c>
       <c r="G26" t="inlineStr">
         <is>
           <t>Não</t>
@@ -1342,7 +1346,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Solicitação de documentação complementar</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1357,19 +1361,15 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Laudiceia</t>
+          <t>Juliana</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>14C5879842FBF191CCE378771DE20033</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Regularização</t>
-        </is>
-      </c>
+          <t>F17621921D038A38C3EB0D53E3733F98</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
           <t>Não</t>
@@ -1379,7 +1379,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Análise para regularização</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1394,12 +1394,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Luciane</t>
+          <t>Laudiceia</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>C54F6E8F93CF6FDCB460C4EC27CB5D0B</t>
+          <t>14C5879842FBF191CCE378771DE20033</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1416,7 +1416,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Análise para regularização</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1436,7 +1436,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>56FEDF1CFCC0CE78021FA9F765943DA5</t>
+          <t>C54F6E8F93CF6FDCB460C4EC27CB5D0B</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1453,7 +1453,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização (2º Relatório)</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1473,7 +1473,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>6B45729139C2A27BC5092915C751010D</t>
+          <t>56FEDF1CFCC0CE78021FA9F765943DA5</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1483,14 +1483,14 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Solicitação de documentação complementar</t>
+          <t>Relatório de conformidades para regularização (2º Relatório)</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1510,20 +1510,24 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2A8C3895F9792659241327C30A81AC6D</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr"/>
+          <t>6B45729139C2A27BC5092915C751010D</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Regularização</t>
+        </is>
+      </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Solicitação de documentação complementar</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1538,19 +1542,15 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Marlei</t>
+          <t>Luciane</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1A97F4E202A341184318AE16C57D676A</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Regularização</t>
-        </is>
-      </c>
+          <t>2A8C3895F9792659241327C30A81AC6D</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
           <t>Não</t>
@@ -1560,7 +1560,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Solicitação de documentação complementar</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1580,10 +1580,14 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>7ACF437DA3089897B5DEF97EE5ADB295</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr"/>
+          <t>1A97F4E202A341184318AE16C57D676A</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Regularização</t>
+        </is>
+      </c>
       <c r="G33" t="inlineStr">
         <is>
           <t>Não</t>
@@ -1593,7 +1597,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Análise para regularização</t>
+          <t>Solicitação de documentação complementar</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1608,19 +1612,15 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Milene</t>
+          <t>Marlei</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>5D79082732416772252230E1D5490EFA</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>Regularização</t>
-        </is>
-      </c>
+          <t>7ACF437DA3089897B5DEF97EE5ADB295</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
           <t>Não</t>
@@ -1630,7 +1630,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Análise para regularização</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1650,7 +1650,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>55DD509716CC263B93E3CBE427D08A02</t>
+          <t>5D79082732416772252230E1D5490EFA</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1682,12 +1682,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Nilda</t>
+          <t>Milene</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>AE754F4FC5F9BFEDC085712FA01026BA</t>
+          <t>55DD509716CC263B93E3CBE427D08A02</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1704,7 +1704,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Solicitação de documentação complementar</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1724,10 +1724,14 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>AF14E2ECA5517720C86670A62C3904DA</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr"/>
+          <t>AE754F4FC5F9BFEDC085712FA01026BA</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Regularização</t>
+        </is>
+      </c>
       <c r="G37" t="inlineStr">
         <is>
           <t>Não</t>
@@ -1737,7 +1741,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Solicitação de documentação complementar</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1752,19 +1756,15 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Peterson</t>
+          <t>Nilda</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>BC998959680EB2D70139D8E84542E2F2</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>Regularização</t>
-        </is>
-      </c>
+          <t>AF14E2ECA5517720C86670A62C3904DA</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
           <t>Não</t>
@@ -1774,7 +1774,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Solicitação de documentação complementar</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1794,10 +1794,14 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>EFDC3F40D59FE406CC2DEF20D8044981</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr"/>
+          <t>BC998959680EB2D70139D8E84542E2F2</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Regularização</t>
+        </is>
+      </c>
       <c r="G39" t="inlineStr">
         <is>
           <t>Não</t>
@@ -1807,7 +1811,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Análise para regularização</t>
+          <t>Solicitação de documentação complementar</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1822,19 +1826,15 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Rosali</t>
+          <t>Peterson</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>B60C7E7F1D99B95E70667D96328CBC70</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>Regularização</t>
-        </is>
-      </c>
+          <t>EFDC3F40D59FE406CC2DEF20D8044981</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
           <t>Não</t>
@@ -1844,7 +1844,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Análise para regularização</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1864,7 +1864,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1981ACD0B95BCA268D57836FFB95AE3A</t>
+          <t>B60C7E7F1D99B95E70667D96328CBC70</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1881,7 +1881,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização (2º Relatório)</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>4B510245B4216AB5086C563FB12FB142</t>
+          <t>1981ACD0B95BCA268D57836FFB95AE3A</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1911,14 +1911,14 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Solicitação de documentação complementar</t>
+          <t>Relatório de conformidades para regularização (2º Relatório)</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1938,20 +1938,24 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>C154AC8381DB0FCD102A1559720175A7</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr"/>
+          <t>4B510245B4216AB5086C563FB12FB142</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Regularização</t>
+        </is>
+      </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Análise para regularização</t>
+          <t>Solicitação de documentação complementar</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1966,19 +1970,15 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Sandra</t>
+          <t>Rosali</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>112D6F0C94649FCED3C07DC35802FB79</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>Regularização</t>
-        </is>
-      </c>
+          <t>C154AC8381DB0FCD102A1559720175A7</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
           <t>Não</t>
@@ -1988,7 +1988,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Análise para regularização</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2008,7 +2008,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>3BC79CA16E0DD94D83CCEF5BE4EFD256</t>
+          <t>112D6F0C94649FCED3C07DC35802FB79</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2025,7 +2025,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Análise para regularização</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2040,12 +2040,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Simone</t>
+          <t>Sandra</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>183830569A2CEF2EEF133D2A68AB051A</t>
+          <t>3BC79CA16E0DD94D83CCEF5BE4EFD256</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2062,7 +2062,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Análise para regularização</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2082,7 +2082,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>B68A9D35C6E7C78C65B895D9B4E8DCBA</t>
+          <t>183830569A2CEF2EEF133D2A68AB051A</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2099,7 +2099,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização (2º Relatório)</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2119,7 +2119,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>866FFD0DE100FC917059EF68503DA039</t>
+          <t>B68A9D35C6E7C78C65B895D9B4E8DCBA</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2129,14 +2129,14 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Solicitação de documentação complementar</t>
+          <t>Relatório de conformidades para regularização (2º Relatório)</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2156,13 +2156,17 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>DB62A611FC09102671B3EA905E42C24C</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr"/>
+          <t>866FFD0DE100FC917059EF68503DA039</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Regularização</t>
+        </is>
+      </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -2184,12 +2188,12 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Vilmar</t>
+          <t>Simone</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>F77DBF14F49FCBA5D570864B9B5782D0</t>
+          <t>DB62A611FC09102671B3EA905E42C24C</t>
         </is>
       </c>
       <c r="F50" t="inlineStr"/>
@@ -2202,32 +2206,32 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para titulação</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ANJO DA GUARDA I</t>
+          <t>ANDER RODOLFO HENRIQUE</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>MANGUEIRINHA</t>
+          <t>DIAMANTE DO OESTE</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>ABEGAIR</t>
+          <t>Valdemar</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>4659B7A30E2601F378DEB2E26CC34160</t>
+          <t>417993C4DBC75A5AFB8702A6E8DF1F2E</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Titulação</t>
+          <t>Regularização</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2239,34 +2243,30 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para titulação</t>
+          <t>Solicitação de documentação complementar</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>ANJO DA GUARDA I</t>
+          <t>ANDER RODOLFO HENRIQUE</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>MANGUEIRINHA</t>
+          <t>DIAMANTE DO OESTE</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>ALICE</t>
+          <t>Valdemar</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>E8E29B0CF7747AD1704653C32DDCBADC</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>Titulação</t>
-        </is>
-      </c>
+          <t>B51387D7D3AACD1978130CE13E6135D2</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
           <t>Não</t>
@@ -2276,34 +2276,30 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para titulação</t>
+          <t>Solicitação de documentação complementar</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>ANJO DA GUARDA I</t>
+          <t>ANDER RODOLFO HENRIQUE</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>MANGUEIRINHA</t>
+          <t>DIAMANTE DO OESTE</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>ANA</t>
+          <t>Vilmar</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>E037A2380B613F045D433F38DE37C94C</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>Titulação</t>
-        </is>
-      </c>
+          <t>F77DBF14F49FCBA5D570864B9B5782D0</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
           <t>Não</t>
@@ -2328,12 +2324,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>AURORA</t>
+          <t>ABEGAIR</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>4455E4BD6D4B48A0769DF97535BECA61</t>
+          <t>4659B7A30E2601F378DEB2E26CC34160</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -2365,12 +2361,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>CLAILTON</t>
+          <t>ALICE</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>FE8F4C07C79E5F59B4EF75F85A873EDD</t>
+          <t>E8E29B0CF7747AD1704653C32DDCBADC</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -2402,12 +2398,12 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>EDINEI</t>
+          <t>ANA</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>125020B35918660F7BB7CFC53190FCB6</t>
+          <t>E037A2380B613F045D433F38DE37C94C</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -2439,12 +2435,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>ELENA</t>
+          <t>AURORA</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>15B79CA41D6EB08ECB182BA3BAE440EB</t>
+          <t>4455E4BD6D4B48A0769DF97535BECA61</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -2476,12 +2472,12 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>ELZA</t>
+          <t>CLAILTON</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>655424431A8B5F3909615336BD17841B</t>
+          <t>FE8F4C07C79E5F59B4EF75F85A873EDD</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -2513,12 +2509,12 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>ENORINA</t>
+          <t>EDINEI</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>3DFD541F6F09F958714D62AF64C1117A</t>
+          <t>125020B35918660F7BB7CFC53190FCB6</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -2550,12 +2546,12 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>IVONE</t>
+          <t>ELENA</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>FB44300B753ABE326562ED9D0D72CE70</t>
+          <t>15B79CA41D6EB08ECB182BA3BAE440EB</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -2587,12 +2583,12 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>JESUVINA</t>
+          <t>ELZA</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>E78E2AA354DE219A0C39E8DC9B6ABC2E</t>
+          <t>655424431A8B5F3909615336BD17841B</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2624,12 +2620,12 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>JOAO</t>
+          <t>ENORINA</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>9807FD589F5FAE6F0B160299B3BF14EF</t>
+          <t>3DFD541F6F09F958714D62AF64C1117A</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -2661,12 +2657,12 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>JOSE</t>
+          <t>IVONE</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2994FFBD435DDC1D01F812137427B9BC</t>
+          <t>FB44300B753ABE326562ED9D0D72CE70</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -2698,12 +2694,12 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>MARIA</t>
+          <t>JESUVINA</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>209746A4FFC3C3338AD57552A1E83BE5</t>
+          <t>E78E2AA354DE219A0C39E8DC9B6ABC2E</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -2735,12 +2731,12 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>MARIA</t>
+          <t>JOAO</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>4D2DF594A01AB6E595524124A4D13559</t>
+          <t>9807FD589F5FAE6F0B160299B3BF14EF</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -2772,12 +2768,12 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>MARILENE</t>
+          <t>JOSE</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>0745C0BB61ACBE83AD0B3EA4A52D05BA</t>
+          <t>2994FFBD435DDC1D01F812137427B9BC</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -2809,12 +2805,12 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>MARLENE</t>
+          <t>MARIA</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>14A7AC36E520550299E9A4CCB6965C71</t>
+          <t>209746A4FFC3C3338AD57552A1E83BE5</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -2846,12 +2842,12 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>MARLI</t>
+          <t>MARIA</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>B0D5862E69F98DA6F7A0661076B8684A</t>
+          <t>4D2DF594A01AB6E595524124A4D13559</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -2883,12 +2879,12 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>NEIVA</t>
+          <t>MARILENE</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>523E7AF091A03C4043D5C9300BC145E2</t>
+          <t>0745C0BB61ACBE83AD0B3EA4A52D05BA</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -2920,12 +2916,12 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>ROSIELI</t>
+          <t>MARLENE</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>97CE285D147B6D4950F8576126FF2790</t>
+          <t>14A7AC36E520550299E9A4CCB6965C71</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -2957,12 +2953,12 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>ROSMARI</t>
+          <t>MARLI</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>5EE88834BE81F9B132B670B4935B2045</t>
+          <t>B0D5862E69F98DA6F7A0661076B8684A</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -2994,12 +2990,12 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>ROZALE</t>
+          <t>NEIVA</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>2E1D277B91BDCBC9123B1408BE73EF95</t>
+          <t>523E7AF091A03C4043D5C9300BC145E2</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -3031,12 +3027,12 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>SANTINA</t>
+          <t>ROSIELI</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>E8F2C4F8144AE6186376F0B243F41A45</t>
+          <t>97CE285D147B6D4950F8576126FF2790</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -3068,12 +3064,12 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>SILVIA</t>
+          <t>ROSMARI</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>FACE3828DD6456398038C0E5DBD30DF2</t>
+          <t>5EE88834BE81F9B132B670B4935B2045</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -3105,12 +3101,12 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>SILVIA</t>
+          <t>ROZALE</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>0C8FF5C5CB7E18BCD7F33CBB8659149B</t>
+          <t>2E1D277B91BDCBC9123B1408BE73EF95</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -3142,12 +3138,12 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>SIVENEI</t>
+          <t>SANTINA</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>5A1DEF016BCD58F9AC8B56E3B0059AF4</t>
+          <t>E8F2C4F8144AE6186376F0B243F41A45</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -3179,12 +3175,12 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>SOELI</t>
+          <t>SILVIA</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>F487ECDF1C33289A90771E483D5F9850</t>
+          <t>FACE3828DD6456398038C0E5DBD30DF2</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -3216,12 +3212,12 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>TEREZINHA</t>
+          <t>SILVIA</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>91B82F46BB6722C855901D73395F74C3</t>
+          <t>0C8FF5C5CB7E18BCD7F33CBB8659149B</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -3253,12 +3249,12 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>VALERIA</t>
+          <t>SIVENEI</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>235625BE6AD69CD5CCD8EEE28070EF97</t>
+          <t>5A1DEF016BCD58F9AC8B56E3B0059AF4</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -3290,12 +3286,12 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>VERA</t>
+          <t>SOELI</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>AAD30565EEE58D53934640A5A0C5217A</t>
+          <t>F487ECDF1C33289A90771E483D5F9850</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -3327,12 +3323,12 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>ZELIA</t>
+          <t>TEREZINHA</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>B8DE5448881F3B1A6AB70F13663A970C</t>
+          <t>91B82F46BB6722C855901D73395F74C3</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -3349,32 +3345,32 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Relatório de conformidades para titulação</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>BANDEIRANTES</t>
+          <t>ANJO DA GUARDA I</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>BANDEIRANTES</t>
+          <t>MANGUEIRINHA</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Fernanda</t>
+          <t>VALERIA</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>F3307895FED7F0D5C2B7A74EEF8C2483</t>
+          <t>235625BE6AD69CD5CCD8EEE28070EF97</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Regularização</t>
+          <t>Titulação</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
@@ -3386,30 +3382,34 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Solicitação de documentação complementar</t>
+          <t>Relatório de conformidades para titulação</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>BANDEIRANTES</t>
+          <t>ANJO DA GUARDA I</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>BANDEIRANTES</t>
+          <t>MANGUEIRINHA</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Fernanda</t>
+          <t>VERA</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>CDF1FCFBB3B12CE4E1D9C160C4ABCA2F</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr"/>
+          <t>AAD30565EEE58D53934640A5A0C5217A</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Titulação</t>
+        </is>
+      </c>
       <c r="G83" t="inlineStr">
         <is>
           <t>Não</t>
@@ -3419,32 +3419,32 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Relatório de conformidades para titulação</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Desconhecido</t>
+          <t>ANJO DA GUARDA I</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Desconhecido</t>
+          <t>MANGUEIRINHA</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Adelar</t>
+          <t>ZELIA</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>98518C564982BC7968097BDEDA2A9BDB</t>
+          <t>B8DE5448881F3B1A6AB70F13663A970C</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Regularização</t>
+          <t>Titulação</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -3461,22 +3461,22 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Desconhecido</t>
+          <t>BANDEIRANTES</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Desconhecido</t>
+          <t>BANDEIRANTES</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Carlos</t>
+          <t>Fernanda</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>5603871BEFECB0AFAB70917123F89B62</t>
+          <t>F3307895FED7F0D5C2B7A74EEF8C2483</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -3493,34 +3493,30 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Solicitação de documentação complementar</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Desconhecido</t>
+          <t>BANDEIRANTES</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Desconhecido</t>
+          <t>BANDEIRANTES</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Gilson</t>
+          <t>Fernanda</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>00ADED1F90850693EC31750E91F6DDDA</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>Regularização</t>
-        </is>
-      </c>
+          <t>CDF1FCFBB3B12CE4E1D9C160C4ABCA2F</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr"/>
       <c r="G86" t="inlineStr">
         <is>
           <t>Não</t>
@@ -3545,12 +3541,12 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Ines</t>
+          <t>Adelar</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>65D4E9AD6E9AD42D5D2AF07D18B2CD4B</t>
+          <t>98518C564982BC7968097BDEDA2A9BDB</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -3567,7 +3563,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Análise para regularização</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -3582,12 +3578,12 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Jorge</t>
+          <t>Carlos</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>809B407CDE2B12254E2C10CA565FA258</t>
+          <t>5603871BEFECB0AFAB70917123F89B62</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -3619,12 +3615,12 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Jorge</t>
+          <t>Gilson</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>2D218C1BFBE8EB50BC25C05DE9FF1CDE</t>
+          <t>00ADED1F90850693EC31750E91F6DDDA</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -3641,7 +3637,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização (2º Relatório)</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -3656,12 +3652,12 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Jorge</t>
+          <t>Ines</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>C2A9E10308768937D00659DB0F499F27</t>
+          <t>65D4E9AD6E9AD42D5D2AF07D18B2CD4B</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -3671,14 +3667,14 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Análise para regularização</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -3693,12 +3689,12 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Soeli</t>
+          <t>Jorge</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>38CDC4B2F0320D2B1A9C254073D919E9</t>
+          <t>809B407CDE2B12254E2C10CA565FA258</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -3730,12 +3726,12 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Valderi</t>
+          <t>Jorge</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>D059819FE574FBA27BD1084144C2533C</t>
+          <t>2D218C1BFBE8EB50BC25C05DE9FF1CDE</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -3752,7 +3748,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Relatório de conformidades para regularização (2º Relatório)</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -3767,12 +3763,12 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Vanessa</t>
+          <t>Jorge</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>78C39F6032417AA9939B72400CFDF106</t>
+          <t>C2A9E10308768937D00659DB0F499F27</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -3782,7 +3778,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -3794,22 +3790,22 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>EDUARDO RADUAN</t>
+          <t>Desconhecido</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>MARMELEIRO</t>
+          <t>Desconhecido</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Ana</t>
+          <t>Soeli</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>66F0D558365A1DA10F1A1FED9BA77CF2</t>
+          <t>38CDC4B2F0320D2B1A9C254073D919E9</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -3831,22 +3827,22 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>EDUARDO RADUAN</t>
+          <t>Desconhecido</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>MARMELEIRO</t>
+          <t>Desconhecido</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Sidinei</t>
+          <t>Valderi</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>70A9ADEC12B287873D1AD48D0C547221</t>
+          <t>D059819FE574FBA27BD1084144C2533C</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -3863,30 +3859,34 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Solicitação de documentação complementar</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>FAZENDA PERSEVERANÇA</t>
+          <t>Desconhecido</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>MARMELEIRO</t>
+          <t>Desconhecido</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Carlos</t>
+          <t>Vanessa</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>A0117E050A1C7FB2BA66C9E8A09E276D</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr"/>
+          <t>78C39F6032417AA9939B72400CFDF106</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Regularização</t>
+        </is>
+      </c>
       <c r="G96" t="inlineStr">
         <is>
           <t>Não</t>
@@ -3901,7 +3901,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>FAZENDA PERSEVERANÇA</t>
+          <t>EDUARDO RADUAN</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3911,12 +3911,12 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Mateus</t>
+          <t>Ana</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>35C1C4254934A59CA02EB17A83B83366</t>
+          <t>66F0D558365A1DA10F1A1FED9BA77CF2</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -3933,12 +3933,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Solicitação de documentação complementar</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>FAZENDA PERSEVERANÇA</t>
+          <t>EDUARDO RADUAN</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3948,15 +3948,19 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Mateus</t>
+          <t>Sidinei</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>6A9A80FECC140C47E666996C67F48185</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr"/>
+          <t>70A9ADEC12B287873D1AD48D0C547221</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Regularização</t>
+        </is>
+      </c>
       <c r="G98" t="inlineStr">
         <is>
           <t>Não</t>
@@ -3966,7 +3970,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Solicitação de documentação complementar</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -3981,19 +3985,15 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Vandressa</t>
+          <t>Carlos</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>6A7BDCE23209F0AE35D1B1405B6E31D8</t>
-        </is>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>Regularização</t>
-        </is>
-      </c>
+          <t>A0117E050A1C7FB2BA66C9E8A09E276D</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr"/>
       <c r="G99" t="inlineStr">
         <is>
           <t>Não</t>
@@ -4003,7 +4003,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Solicitação de documentação complementar</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -4018,15 +4018,19 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Vandressa</t>
+          <t>Mateus</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>4A9BD6FEB4126E745C70109123AC2FF2</t>
-        </is>
-      </c>
-      <c r="F100" t="inlineStr"/>
+          <t>35C1C4254934A59CA02EB17A83B83366</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>Regularização</t>
+        </is>
+      </c>
       <c r="G100" t="inlineStr">
         <is>
           <t>Não</t>
@@ -4036,34 +4040,30 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para titulação</t>
+          <t>Solicitação de documentação complementar</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>MARCOS FREIRE</t>
+          <t>FAZENDA PERSEVERANÇA</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>RIO BONITO DO IGUACU</t>
+          <t>MARMELEIRO</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>ADAO</t>
+          <t>Mateus</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>014BAB36F8CB0E3974B4D3EC3DA67634</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>Titulação</t>
-        </is>
-      </c>
+          <t>6A9A80FECC140C47E666996C67F48185</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr"/>
       <c r="G101" t="inlineStr">
         <is>
           <t>Não</t>
@@ -4073,32 +4073,32 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para titulação</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>MARCOS FREIRE</t>
+          <t>FAZENDA PERSEVERANÇA</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>RIO BONITO DO IGUACU</t>
+          <t>MARMELEIRO</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>ADELMO</t>
+          <t>Vandressa</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>B1D7D4C55F3632708DAF7A11F625069D</t>
+          <t>6A7BDCE23209F0AE35D1B1405B6E31D8</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Titulação</t>
+          <t>Regularização</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
@@ -4110,34 +4110,30 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para titulação</t>
+          <t>Solicitação de documentação complementar</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>MARCOS FREIRE</t>
+          <t>FAZENDA PERSEVERANÇA</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>RIO BONITO DO IGUACU</t>
+          <t>MARMELEIRO</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>ADRIANE</t>
+          <t>Vandressa</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>E1EFAD895566A0F831CC975AFFD6BE72</t>
-        </is>
-      </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>Titulação</t>
-        </is>
-      </c>
+          <t>4A9BD6FEB4126E745C70109123AC2FF2</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr"/>
       <c r="G103" t="inlineStr">
         <is>
           <t>Não</t>
@@ -4162,12 +4158,12 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>ADRIANO</t>
+          <t>ADAO</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>435804F17C048647DBCF7293E4203BD6</t>
+          <t>014BAB36F8CB0E3974B4D3EC3DA67634</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -4199,12 +4195,12 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>ALEDIR</t>
+          <t>ADELMO</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>03B9CA051196BD5D701A33BDC15CD539</t>
+          <t>B1D7D4C55F3632708DAF7A11F625069D</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -4236,12 +4232,12 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>ALTIDOR</t>
+          <t>ADRIANE</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>FDE7919B6759EF9A9C4BE21E</t>
+          <t>E1EFAD895566A0F831CC975AFFD6BE72</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -4273,12 +4269,12 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>AMARILDO</t>
+          <t>ADRIANO</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>35ACBB8EBE445EC62AE84B9241C1D840</t>
+          <t>435804F17C048647DBCF7293E4203BD6</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -4310,12 +4306,12 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>AMAURI</t>
+          <t>ALEDIR</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>A35AB902B32CF8BDCF9EB71F521CFA46</t>
+          <t>03B9CA051196BD5D701A33BDC15CD539</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -4347,12 +4343,12 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>ANA</t>
+          <t>ALTIDOR</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>EA5217E5C084E59EAE8A6C2AA044310E</t>
+          <t>FDE7919B6759EF9A9C4BE21E</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -4384,12 +4380,12 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>ANDRE</t>
+          <t>AMARILDO</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>8D667040D470EA3BC965931E</t>
+          <t>35ACBB8EBE445EC62AE84B9241C1D840</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -4421,12 +4417,12 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>ANDREI</t>
+          <t>AMAURI</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>CFC10F9DE33CBC91485B143BAE6BEC58</t>
+          <t>A35AB902B32CF8BDCF9EB71F521CFA46</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -4458,12 +4454,12 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>ANDRESA</t>
+          <t>ANA</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>A1DB26C8961C29C557DD82714A5AE9DD</t>
+          <t>EA5217E5C084E59EAE8A6C2AA044310E</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -4495,12 +4491,12 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>ANTONIO</t>
+          <t>ANDRE</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>58F188E7D70832A4700CE195</t>
+          <t>8D667040D470EA3BC965931E</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -4532,12 +4528,12 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>ARI</t>
+          <t>ANDREI</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>A266E3C437EC493A2E7592743F9F605D</t>
+          <t>CFC10F9DE33CBC91485B143BAE6BEC58</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -4569,12 +4565,12 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>CARLOS</t>
+          <t>ANDRESA</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>2899E8F3CC332BD0DFB530AEB5930BBC</t>
+          <t>A1DB26C8961C29C557DD82714A5AE9DD</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -4606,12 +4602,12 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>CLEUNIR</t>
+          <t>ANTONIO</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>E9EA2B28A0593A9CBFF504EF</t>
+          <t>58F188E7D70832A4700CE195</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -4643,12 +4639,12 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>CLEUSMERE</t>
+          <t>ARI</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>36C1BF6A0B5B4EB53752A2B13558AFE0</t>
+          <t>A266E3C437EC493A2E7592743F9F605D</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -4680,12 +4676,12 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>CREZOLINA</t>
+          <t>CARLOS</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>2A4397DE68D8075CE4C924196B95CFE1</t>
+          <t>2899E8F3CC332BD0DFB530AEB5930BBC</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -4717,12 +4713,12 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>DALMO</t>
+          <t>CLEUNIR</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>C8E81BC5A10922EE9C0A2DAC104CAB53</t>
+          <t>E9EA2B28A0593A9CBFF504EF</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -4754,12 +4750,12 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>DEBRA</t>
+          <t>CLEUSMERE</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>15846C0DF7AAF89C173C8848</t>
+          <t>36C1BF6A0B5B4EB53752A2B13558AFE0</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -4791,12 +4787,12 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>DOMINGOS</t>
+          <t>CREZOLINA</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>023AB3CC001228BC5C78D6DE47A089BF</t>
+          <t>2A4397DE68D8075CE4C924196B95CFE1</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -4828,12 +4824,12 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>EGINO</t>
+          <t>DALMO</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>C3082229B0D7CF513C2F50F741236CE1</t>
+          <t>C8E81BC5A10922EE9C0A2DAC104CAB53</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -4865,12 +4861,12 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>ELIAS</t>
+          <t>DEBRA</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>80AC8030BFF2207AFE5C641DC1228308</t>
+          <t>15846C0DF7AAF89C173C8848</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -4902,12 +4898,12 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>ELOIR</t>
+          <t>DOMINGOS</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>C61CADE2ED4EE9A29FA9A771765E568B</t>
+          <t>023AB3CC001228BC5C78D6DE47A089BF</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -4939,12 +4935,12 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>EMILIA</t>
+          <t>EGINO</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>5849C202A865C8DA</t>
+          <t>C3082229B0D7CF513C2F50F741236CE1</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -4976,12 +4972,12 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>ESMERALDO</t>
+          <t>ELIAS</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>B70093BB744DECFE135A97385DF281B3</t>
+          <t>80AC8030BFF2207AFE5C641DC1228308</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -5013,12 +5009,12 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>EVA</t>
+          <t>ELOIR</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>B53D642DE3BD0515FC91DFF9</t>
+          <t>C61CADE2ED4EE9A29FA9A771765E568B</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -5050,12 +5046,12 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>EVANIR</t>
+          <t>EMILIA</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>267FF1F6A1BCD73DB1D9D0ADA51AAEF6</t>
+          <t>5849C202A865C8DA</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -5087,12 +5083,12 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>FLAVIA</t>
+          <t>ESMERALDO</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>2A57C76ED89EEFEA15A976ADF2F4781C</t>
+          <t>B70093BB744DECFE135A97385DF281B3</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -5124,12 +5120,12 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>FRANCIELI</t>
+          <t>EVA</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>DAEF2AD926A2B4EB8EB4C56D5463F646</t>
+          <t>B53D642DE3BD0515FC91DFF9</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -5161,12 +5157,12 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>GILMAR</t>
+          <t>EVANIR</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>1E8240C317FFA21814EA4826AEF409B9</t>
+          <t>267FF1F6A1BCD73DB1D9D0ADA51AAEF6</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -5198,12 +5194,12 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>GLORIA</t>
+          <t>FLAVIA</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>591DAE110B436D51CC6928D3702BA1F8</t>
+          <t>2A57C76ED89EEFEA15A976ADF2F4781C</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -5235,12 +5231,12 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>HILARIO</t>
+          <t>FRANCIELI</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>9976454DF3F3166A83B8F0C704008AB1</t>
+          <t>DAEF2AD926A2B4EB8EB4C56D5463F646</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -5272,12 +5268,12 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>ILARIO</t>
+          <t>GILMAR</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>58D6EA764BEC5BC4BF7EABE58C7199AD</t>
+          <t>1E8240C317FFA21814EA4826AEF409B9</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -5309,12 +5305,12 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>INES</t>
+          <t>GLORIA</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>530CF447A29FC6961A49A0DFA1DF0F40</t>
+          <t>591DAE110B436D51CC6928D3702BA1F8</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -5346,12 +5342,12 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>IRACIDE</t>
+          <t>HILARIO</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>6583EF3F9EC67EC1B67B7609</t>
+          <t>9976454DF3F3166A83B8F0C704008AB1</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -5383,12 +5379,12 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>IRACILDE</t>
+          <t>ILARIO</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>57B51F2B28E0E13A333B8A85</t>
+          <t>58D6EA764BEC5BC4BF7EABE58C7199AD</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -5420,12 +5416,12 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>IRINEU</t>
+          <t>INES</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>0C1C208288BB698047B0DFC37B7FB3D9</t>
+          <t>530CF447A29FC6961A49A0DFA1DF0F40</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -5457,12 +5453,12 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>IRONI</t>
+          <t>IRACIDE</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>1A331663D155C747E23A40C0</t>
+          <t>6583EF3F9EC67EC1B67B7609</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -5494,12 +5490,12 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>IVETE</t>
+          <t>IRACILDE</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>8C9D6BA0F9EA40D362B6124E962ED22E</t>
+          <t>57B51F2B28E0E13A333B8A85</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -5531,12 +5527,12 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>IZOLINA</t>
+          <t>IRINEU</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>E8311641DD7356CA67855B70815D9859</t>
+          <t>0C1C208288BB698047B0DFC37B7FB3D9</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -5568,12 +5564,12 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>JILSON</t>
+          <t>IRONI</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>4CA428A3EAC673AAFDBEF1636A12CA17</t>
+          <t>1A331663D155C747E23A40C0</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -5605,12 +5601,12 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>JOAO</t>
+          <t>IVETE</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>120C7899FEE3C6579152DBD4</t>
+          <t>8C9D6BA0F9EA40D362B6124E962ED22E</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -5642,12 +5638,12 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>JOAQUIM</t>
+          <t>IZOLINA</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>40EBCBBFAB5A1EC1DB67AA5725F2B026</t>
+          <t>E8311641DD7356CA67855B70815D9859</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -5679,12 +5675,12 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>JORGE</t>
+          <t>JILSON</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>63C0EB546AA0E8525A7606F839430BD5</t>
+          <t>4CA428A3EAC673AAFDBEF1636A12CA17</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -5716,12 +5712,12 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>JOSE</t>
+          <t>JOAO</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>B93DF3590401ADB0124B7B426BA573D1</t>
+          <t>120C7899FEE3C6579152DBD4</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -5753,12 +5749,12 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>JOSILENE</t>
+          <t>JOAQUIM</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>B014E612149D2006410E59E4F311B062</t>
+          <t>40EBCBBFAB5A1EC1DB67AA5725F2B026</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -5790,12 +5786,12 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>JULIO</t>
+          <t>JORGE</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>76D9BA95E9C84BA95BF126BCA99A9AA9</t>
+          <t>63C0EB546AA0E8525A7606F839430BD5</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -5827,12 +5823,12 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>LEONARDO</t>
+          <t>JOSE</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>0B41EE7BE4281E63D58B11F3B8FEB055</t>
+          <t>B93DF3590401ADB0124B7B426BA573D1</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -5864,12 +5860,12 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>LUIZ</t>
+          <t>JOSILENE</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>C793E56EFE371E0712981CAB2602CDDE</t>
+          <t>B014E612149D2006410E59E4F311B062</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -5901,12 +5897,12 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>MARCILIO</t>
+          <t>JULIO</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>7475D48F01F271414EABB477303B2735</t>
+          <t>76D9BA95E9C84BA95BF126BCA99A9AA9</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -5938,12 +5934,12 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>MARIA</t>
+          <t>LEONARDO</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>8DDEB4F9760987B92279CC48</t>
+          <t>0B41EE7BE4281E63D58B11F3B8FEB055</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -5975,12 +5971,12 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>MARIA</t>
+          <t>LUIZ</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>AD4CD742CA930B61</t>
+          <t>C793E56EFE371E0712981CAB2602CDDE</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -6012,12 +6008,12 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>MAURICIO</t>
+          <t>MARCILIO</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>99E6FE7324EF6FFA3BB063D2C868946B</t>
+          <t>7475D48F01F271414EABB477303B2735</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -6049,12 +6045,12 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>MIGUEL</t>
+          <t>MARIA</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>8D233C11EAAABA4D8A8CE025C13D31CD</t>
+          <t>8DDEB4F9760987B92279CC48</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -6086,12 +6082,12 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>MILTON</t>
+          <t>MARIA</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>65942DD6FFC0EE274CCBD1A6C3EFFFF5</t>
+          <t>AD4CD742CA930B61</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -6123,12 +6119,12 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>NERI</t>
+          <t>MAURICIO</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>F42DD84280AE898E757D84D2E9F472CD</t>
+          <t>99E6FE7324EF6FFA3BB063D2C868946B</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -6160,12 +6156,12 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>NERIVANI</t>
+          <t>MIGUEL</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>CCEABCD76CD04AA74B01F1BF0493082E</t>
+          <t>8D233C11EAAABA4D8A8CE025C13D31CD</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -6197,12 +6193,12 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>NILTON</t>
+          <t>MILTON</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>8EB91B8D2B2E04B30FDE95E2470826D9</t>
+          <t>65942DD6FFC0EE274CCBD1A6C3EFFFF5</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -6234,12 +6230,12 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>ODAIR</t>
+          <t>NERI</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>0E61191DDCB2E017A4BF5B25</t>
+          <t>F42DD84280AE898E757D84D2E9F472CD</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -6271,12 +6267,12 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>ODILON</t>
+          <t>NERIVANI</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>F4831649F90BE10AA5B8A15EC3A664B2</t>
+          <t>CCEABCD76CD04AA74B01F1BF0493082E</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -6308,12 +6304,12 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>ODIR</t>
+          <t>NILTON</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>ED924C1703207F58C226ABD2BA894DC1</t>
+          <t>8EB91B8D2B2E04B30FDE95E2470826D9</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -6345,12 +6341,12 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>ORLEI</t>
+          <t>ODAIR</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>FB138AA0FBB43A5DF6DD4BB50AE45870</t>
+          <t>0E61191DDCB2E017A4BF5B25</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -6382,12 +6378,12 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>PAULO</t>
+          <t>ODILON</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>654A36C55A7A1D234064B5A150C66FEF</t>
+          <t>F4831649F90BE10AA5B8A15EC3A664B2</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -6419,12 +6415,12 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>PEDRO</t>
+          <t>ODIR</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>0886B84EF904DD7B7596DA309703D0F5</t>
+          <t>ED924C1703207F58C226ABD2BA894DC1</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -6456,12 +6452,12 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>PEDRO</t>
+          <t>ORLEI</t>
         </is>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>C222D7A9E0E0AFBFB7E45B03</t>
+          <t>FB138AA0FBB43A5DF6DD4BB50AE45870</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -6493,12 +6489,12 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>RAMILIO</t>
+          <t>PAULO</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>807265C0454852BA53A79CDADC28E736</t>
+          <t>654A36C55A7A1D234064B5A150C66FEF</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -6530,12 +6526,12 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>RICHARDE</t>
+          <t>PEDRO</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>EE90CB435A0F0F5688C31C5734E45864</t>
+          <t>0886B84EF904DD7B7596DA309703D0F5</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -6567,12 +6563,12 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>RISONEIDE</t>
+          <t>PEDRO</t>
         </is>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>62D7F5DA2D9208AEECE1E82D</t>
+          <t>C222D7A9E0E0AFBFB7E45B03</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -6604,12 +6600,12 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>ROSANE</t>
+          <t>RAMILIO</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>DC98DD629486BBE60096FD8F</t>
+          <t>807265C0454852BA53A79CDADC28E736</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -6641,12 +6637,12 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>ROSELI</t>
+          <t>RICHARDE</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>1688F39642A8A4E06AE623BA</t>
+          <t>EE90CB435A0F0F5688C31C5734E45864</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -6678,12 +6674,12 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>ROSILEI</t>
+          <t>RISONEIDE</t>
         </is>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>23FCBDBD8A17FC8EF61FB334FD963002</t>
+          <t>62D7F5DA2D9208AEECE1E82D</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -6715,12 +6711,12 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>SANDRA</t>
+          <t>ROSANE</t>
         </is>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>C4AF5B6C1763061DA4404FAB647B474A</t>
+          <t>DC98DD629486BBE60096FD8F</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -6752,12 +6748,12 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>SERGIO</t>
+          <t>ROSELI</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>5AF5202624AA851F0618548C4848A4AE</t>
+          <t>1688F39642A8A4E06AE623BA</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -6789,12 +6785,12 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>SOLANGE</t>
+          <t>ROSILEI</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>49971DF5A6A1886DEA2B3BCB2BDC7A22</t>
+          <t>23FCBDBD8A17FC8EF61FB334FD963002</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -6826,12 +6822,12 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>SOLANGE</t>
+          <t>SANDRA</t>
         </is>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>0B5B7F20B3AAF66B3B11AFE2690CA8FF</t>
+          <t>C4AF5B6C1763061DA4404FAB647B474A</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -6863,12 +6859,12 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>TERESA</t>
+          <t>SERGIO</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>79F85F694A43544B6A80F8EEEADEE33B</t>
+          <t>5AF5202624AA851F0618548C4848A4AE</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -6900,12 +6896,12 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>VAGNER</t>
+          <t>SOLANGE</t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>054C62B69E7F11FCD7A625EFA87F7B64</t>
+          <t>49971DF5A6A1886DEA2B3BCB2BDC7A22</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -6937,12 +6933,12 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>VALDECIR</t>
+          <t>SOLANGE</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>3AF27C20C44C67BCD6AB41CA</t>
+          <t>0B5B7F20B3AAF66B3B11AFE2690CA8FF</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -6974,12 +6970,12 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>VALDECIR</t>
+          <t>TERESA</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>36E63A5F9DA84577A287AB3AD7838570</t>
+          <t>79F85F694A43544B6A80F8EEEADEE33B</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
@@ -7011,12 +7007,12 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>VALDECIR</t>
+          <t>VAGNER</t>
         </is>
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>3E1E4FE810431C4FAF864692F4496356</t>
+          <t>054C62B69E7F11FCD7A625EFA87F7B64</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
@@ -7048,12 +7044,12 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>VALDELIR</t>
+          <t>VALDECIR</t>
         </is>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>4A67F2639BF3A22A</t>
+          <t>3AF27C20C44C67BCD6AB41CA</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -7085,12 +7081,12 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>VALDEMAR</t>
+          <t>VALDECIR</t>
         </is>
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>19CEF982DA697F35F531B1DAFC8F7736</t>
+          <t>36E63A5F9DA84577A287AB3AD7838570</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -7122,12 +7118,12 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>VALMOR</t>
+          <t>VALDECIR</t>
         </is>
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>0B73B73D62DFDE7539EF7D58EE0FD900</t>
+          <t>3E1E4FE810431C4FAF864692F4496356</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
@@ -7159,12 +7155,12 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>VERA</t>
+          <t>VALDELIR</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>4AE8DF88CA22D75D3B87C078E601B5BA</t>
+          <t>4A67F2639BF3A22A</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
@@ -7196,12 +7192,12 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>VERA</t>
+          <t>VALDEMAR</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>7D9410A51C9BECD98BE4AB73CCFF94EF</t>
+          <t>19CEF982DA697F35F531B1DAFC8F7736</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -7233,12 +7229,12 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>VIVALDINO</t>
+          <t>VALMOR</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>C573D9CB02AD42FB2BA99478</t>
+          <t>0B73B73D62DFDE7539EF7D58EE0FD900</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
@@ -7270,12 +7266,12 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>ZELI</t>
+          <t>VERA</t>
         </is>
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>ABAD0132624D7093B20B4BD8E232D5D4</t>
+          <t>4AE8DF88CA22D75D3B87C078E601B5BA</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -7292,32 +7288,32 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Análise para regularização</t>
+          <t>Relatório de conformidades para titulação</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>ROSELI NUNES</t>
+          <t>MARCOS FREIRE</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>SAO JERONIMO DA SERRA</t>
+          <t>RIO BONITO DO IGUACU</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>Guilherme</t>
+          <t>VERA</t>
         </is>
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>4C91EE4CEE2814F5667059FBECB733FC</t>
+          <t>7D9410A51C9BECD98BE4AB73CCFF94EF</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
         <is>
-          <t>Regularização</t>
+          <t>Titulação</t>
         </is>
       </c>
       <c r="G189" t="inlineStr">
@@ -7329,32 +7325,32 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para regularização</t>
+          <t>Relatório de conformidades para titulação</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>ROSELI NUNES</t>
+          <t>MARCOS FREIRE</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>SAO JERONIMO DA SERRA</t>
+          <t>RIO BONITO DO IGUACU</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>Guilherme</t>
+          <t>VIVALDINO</t>
         </is>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>B53F099B4CC28D9A9292715B93005CED</t>
+          <t>C573D9CB02AD42FB2BA99478</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
         <is>
-          <t>Regularização</t>
+          <t>Titulação</t>
         </is>
       </c>
       <c r="G190" t="inlineStr">
@@ -7371,22 +7367,22 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>SÃO JOÃO MARIA</t>
+          <t>MARCOS FREIRE</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>MANGUEIRINHA</t>
+          <t>RIO BONITO DO IGUACU</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>ALGEO</t>
+          <t>ZELI</t>
         </is>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>80D3B91F0216135B589BD5134F748BE4</t>
+          <t>ABAD0132624D7093B20B4BD8E232D5D4</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -7403,32 +7399,32 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para titulação</t>
+          <t>Análise para regularização</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>SÃO JOÃO MARIA</t>
+          <t>ROSELI NUNES</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>MANGUEIRINHA</t>
+          <t>SAO JERONIMO DA SERRA</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>CATIANE</t>
+          <t>Guilherme</t>
         </is>
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>313BF2A9C5097FEFFA6D111181AAC4C6</t>
+          <t>4C91EE4CEE2814F5667059FBECB733FC</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
         <is>
-          <t>Titulação</t>
+          <t>Regularização</t>
         </is>
       </c>
       <c r="G192" t="inlineStr">
@@ -7440,32 +7436,32 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Relatório de conformidades para titulação</t>
+          <t>Relatório de conformidades para regularização</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>SÃO JOÃO MARIA</t>
+          <t>ROSELI NUNES</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>MANGUEIRINHA</t>
+          <t>SAO JERONIMO DA SERRA</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>ELIANA</t>
+          <t>Guilherme</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>4EC1DF1919FB1C6A2E61932168F1FEC4</t>
+          <t>B53F099B4CC28D9A9292715B93005CED</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
         <is>
-          <t>Titulação</t>
+          <t>Regularização</t>
         </is>
       </c>
       <c r="G193" t="inlineStr">
@@ -7492,12 +7488,12 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>EVANDRO</t>
+          <t>ALGEO</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>D878A8A453365E4F339D6A70EDB8BE5F</t>
+          <t>80D3B91F0216135B589BD5134F748BE4</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -7529,12 +7525,12 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>IZABEL</t>
+          <t>CATIANE</t>
         </is>
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>6BC9955D6D4517F542719718ADBB5CBA</t>
+          <t>313BF2A9C5097FEFFA6D111181AAC4C6</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
@@ -7566,12 +7562,12 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>JULIANA</t>
+          <t>ELIANA</t>
         </is>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>AA6394BAB4043191E564E776EC94F4C6</t>
+          <t>4EC1DF1919FB1C6A2E61932168F1FEC4</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -7603,12 +7599,12 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>LORENI</t>
+          <t>EVANDRO</t>
         </is>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>999B529D8030164D1E16CE7F3496EC60</t>
+          <t>D878A8A453365E4F339D6A70EDB8BE5F</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -7640,12 +7636,12 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>LUANA</t>
+          <t>IZABEL</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>51CAF6761F8B63C53F18AADA77CF47C9</t>
+          <t>6BC9955D6D4517F542719718ADBB5CBA</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -7677,12 +7673,12 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>MARIA</t>
+          <t>JULIANA</t>
         </is>
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>C440E6C136BB58D379DE9883737840BD</t>
+          <t>AA6394BAB4043191E564E776EC94F4C6</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
@@ -7714,12 +7710,12 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>MARIA</t>
+          <t>LORENI</t>
         </is>
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>08805B016AF8931C656D00E6E80B9466</t>
+          <t>999B529D8030164D1E16CE7F3496EC60</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
@@ -7751,12 +7747,12 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>MARIA</t>
+          <t>LUANA</t>
         </is>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>D65A19FFE192E628CE690DB63B90862E</t>
+          <t>51CAF6761F8B63C53F18AADA77CF47C9</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -7793,7 +7789,7 @@
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>B4EA879215CFC5260D19A24205CFA111</t>
+          <t>C440E6C136BB58D379DE9883737840BD</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -7830,7 +7826,7 @@
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>FF15CA7EE716FCAC990751FAFDBEEEEC</t>
+          <t>08805B016AF8931C656D00E6E80B9466</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -7862,12 +7858,12 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>MARLENE</t>
+          <t>MARIA</t>
         </is>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>B00D5B9FA91B68F970242DCD9F0A2DCC</t>
+          <t>D65A19FFE192E628CE690DB63B90862E</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
@@ -7899,12 +7895,12 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>NANCI</t>
+          <t>MARIA</t>
         </is>
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>7ED6ADA5B005BD1EA7FC7C29E8D8EEDA</t>
+          <t>B4EA879215CFC5260D19A24205CFA111</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -7936,12 +7932,12 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>REGINA</t>
+          <t>MARIA</t>
         </is>
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>25786A793A5E92E236C386E5EA1A111E</t>
+          <t>FF15CA7EE716FCAC990751FAFDBEEEEC</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -7973,12 +7969,12 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>ROMILDA</t>
+          <t>MARLENE</t>
         </is>
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>44B922FE7347C3BD1F6E071D9FCD5B3E</t>
+          <t>B00D5B9FA91B68F970242DCD9F0A2DCC</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -8010,12 +8006,12 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>SONIA</t>
+          <t>NANCI</t>
         </is>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>3AFD839D7CD5A2D302FF80ECD7C722FA</t>
+          <t>7ED6ADA5B005BD1EA7FC7C29E8D8EEDA</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -8047,12 +8043,12 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>TAILSA</t>
+          <t>REGINA</t>
         </is>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>E53D810CA1A5D031192DC175E8881B21</t>
+          <t>25786A793A5E92E236C386E5EA1A111E</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -8084,12 +8080,12 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>TEREZINHA</t>
+          <t>ROMILDA</t>
         </is>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>F6CF1DA014356D45EC15E37A4CAD9891</t>
+          <t>44B922FE7347C3BD1F6E071D9FCD5B3E</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -8121,12 +8117,12 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>TEREZINHA</t>
+          <t>SONIA</t>
         </is>
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>4D9C66485D8CF7DBC3E43B8472D1E365</t>
+          <t>3AFD839D7CD5A2D302FF80ECD7C722FA</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -8158,20 +8154,131 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
+          <t>TAILSA</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>E53D810CA1A5D031192DC175E8881B21</t>
+        </is>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>Titulação</t>
+        </is>
+      </c>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>Relatório de conformidades para titulação</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>SÃO JOÃO MARIA</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>MANGUEIRINHA</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
           <t>TEREZINHA</t>
         </is>
       </c>
-      <c r="E212" t="inlineStr">
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>F6CF1DA014356D45EC15E37A4CAD9891</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>Titulação</t>
+        </is>
+      </c>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>Relatório de conformidades para titulação</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>SÃO JOÃO MARIA</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>MANGUEIRINHA</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>TEREZINHA</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>4D9C66485D8CF7DBC3E43B8472D1E365</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>Titulação</t>
+        </is>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>Relatório de conformidades para titulação</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>SÃO JOÃO MARIA</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>MANGUEIRINHA</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>TEREZINHA</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
         <is>
           <t>CEB80B59A443673B14CFDA604C151E3F</t>
         </is>
       </c>
-      <c r="F212" t="inlineStr">
-        <is>
-          <t>Titulação</t>
-        </is>
-      </c>
-      <c r="G212" t="inlineStr">
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>Titulação</t>
+        </is>
+      </c>
+      <c r="G215" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
@@ -8438,13 +8545,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A05C52C-7D9D-42D0-A125-8BC83E2C47E0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D09EE3A-9EDD-40C1-A905-6300525DFAD3}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37BD57F6-027E-495D-837F-13976FDE58A9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B979BABB-F04D-4DA5-8F5B-76FA35A04A20}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FEAA85B-3FEF-48F0-A500-7E44938EDA80}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC8FB53A-C0AB-4638-9E80-3EA290FB0AD7}"/>
 </file>
</xml_diff>